<commit_message>
updated with extra calcs
</commit_message>
<xml_diff>
--- a/Data Exploration.xlsx
+++ b/Data Exploration.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10814"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="M:\Github-Version-Control-Projects\BioHEART\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matthewshu/Documents/GitHub Projects/BioHEART-Biological-Age/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6749428B-A805-4120-A41B-ED6184304C9B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2702E702-135C-644C-8E1F-6DC775C5B9C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3825" yWindow="2505" windowWidth="31485" windowHeight="16080" xr2:uid="{DC4E264E-888D-42B0-BAF1-131E9CBAF4F4}"/>
+    <workbookView xWindow="0" yWindow="600" windowWidth="28800" windowHeight="16080" xr2:uid="{DC4E264E-888D-42B0-BAF1-131E9CBAF4F4}"/>
   </bookViews>
   <sheets>
     <sheet name="MetabAge Variables Required" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,6 @@
     <definedName name="teacher_description_7" localSheetId="0">'MetabAge Variables Required'!$K$2:$CI$2</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -2854,252 +2853,250 @@
   <dimension ref="A1:K260"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+      <selection activeCell="I22" sqref="I22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="2" width="26.85546875" customWidth="1"/>
-    <col min="3" max="3" width="46.140625" customWidth="1"/>
+    <col min="1" max="2" width="26.83203125" customWidth="1"/>
+    <col min="3" max="3" width="46.1640625" customWidth="1"/>
     <col min="5" max="5" width="0" hidden="1" customWidth="1"/>
-    <col min="8" max="8" width="28.28515625" customWidth="1"/>
-    <col min="9" max="9" width="38.42578125" customWidth="1"/>
+    <col min="8" max="8" width="28.33203125" customWidth="1"/>
+    <col min="9" max="9" width="38.5" customWidth="1"/>
     <col min="10" max="10" width="24" customWidth="1"/>
-    <col min="11" max="11" width="33.28515625" customWidth="1"/>
-    <col min="12" max="12" width="6.42578125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="6.5703125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="7.140625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="16" max="18" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="33.33203125" customWidth="1"/>
+    <col min="12" max="13" width="6.5" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="7.1640625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="16" max="18" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="12.83203125" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="11" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="12.1640625" bestFit="1" customWidth="1"/>
     <col min="26" max="26" width="18" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="21.42578125" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="22.140625" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="21.5" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="16.5" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="22.1640625" bestFit="1" customWidth="1"/>
     <col min="30" max="30" width="19" bestFit="1" customWidth="1"/>
-    <col min="31" max="33" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="31" max="33" width="18.1640625" bestFit="1" customWidth="1"/>
     <col min="34" max="34" width="22" bestFit="1" customWidth="1"/>
-    <col min="35" max="36" width="18.28515625" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="19.28515625" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="18.5703125" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="25.7109375" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="17.85546875" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="44" max="44" width="18.28515625" bestFit="1" customWidth="1"/>
-    <col min="45" max="45" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="46" max="48" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="49" max="50" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="51" max="51" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="52" max="52" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="35" max="36" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="19.33203125" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="18.5" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="17.5" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="25.6640625" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="17.83203125" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="46" max="48" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="49" max="50" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="51" max="51" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="52" max="52" width="11.6640625" bestFit="1" customWidth="1"/>
     <col min="53" max="53" width="21" bestFit="1" customWidth="1"/>
-    <col min="54" max="54" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="55" max="55" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="56" max="58" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="59" max="60" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="61" max="61" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="62" max="62" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="63" max="63" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="64" max="64" width="25.7109375" bestFit="1" customWidth="1"/>
-    <col min="65" max="65" width="30.85546875" bestFit="1" customWidth="1"/>
+    <col min="54" max="54" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="55" max="55" width="16.5" bestFit="1" customWidth="1"/>
+    <col min="56" max="58" width="13.1640625" bestFit="1" customWidth="1"/>
+    <col min="59" max="60" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="61" max="61" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="62" max="62" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="63" max="63" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="64" max="64" width="25.6640625" bestFit="1" customWidth="1"/>
+    <col min="65" max="65" width="30.83203125" bestFit="1" customWidth="1"/>
     <col min="66" max="66" width="21" bestFit="1" customWidth="1"/>
-    <col min="67" max="67" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="68" max="68" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="69" max="69" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="70" max="70" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="71" max="71" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="72" max="72" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="73" max="73" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="67" max="68" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="69" max="69" width="16.5" bestFit="1" customWidth="1"/>
+    <col min="70" max="70" width="15.1640625" bestFit="1" customWidth="1"/>
+    <col min="71" max="71" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="72" max="72" width="16.5" bestFit="1" customWidth="1"/>
+    <col min="73" max="73" width="10.5" bestFit="1" customWidth="1"/>
     <col min="74" max="74" width="11" bestFit="1" customWidth="1"/>
     <col min="75" max="75" width="17" bestFit="1" customWidth="1"/>
-    <col min="76" max="76" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="77" max="77" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="78" max="79" width="22.28515625" bestFit="1" customWidth="1"/>
-    <col min="80" max="80" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="81" max="81" width="22.85546875" bestFit="1" customWidth="1"/>
-    <col min="82" max="82" width="21.42578125" bestFit="1" customWidth="1"/>
-    <col min="83" max="85" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="86" max="86" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="87" max="87" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="88" max="88" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="89" max="89" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="90" max="90" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="91" max="91" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="76" max="76" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="77" max="77" width="16.5" bestFit="1" customWidth="1"/>
+    <col min="78" max="79" width="22.33203125" bestFit="1" customWidth="1"/>
+    <col min="80" max="80" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="81" max="81" width="22.83203125" bestFit="1" customWidth="1"/>
+    <col min="82" max="82" width="21.5" bestFit="1" customWidth="1"/>
+    <col min="83" max="85" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="86" max="86" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="87" max="87" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="88" max="88" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="89" max="89" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="90" max="90" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="91" max="91" width="18.5" bestFit="1" customWidth="1"/>
     <col min="92" max="92" width="3" bestFit="1" customWidth="1"/>
-    <col min="93" max="93" width="4.140625" bestFit="1" customWidth="1"/>
-    <col min="94" max="94" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="93" max="93" width="4.1640625" bestFit="1" customWidth="1"/>
+    <col min="94" max="94" width="6.1640625" bestFit="1" customWidth="1"/>
     <col min="95" max="95" width="6" bestFit="1" customWidth="1"/>
     <col min="96" max="96" width="3" bestFit="1" customWidth="1"/>
-    <col min="97" max="97" width="7.140625" bestFit="1" customWidth="1"/>
+    <col min="97" max="97" width="7.1640625" bestFit="1" customWidth="1"/>
     <col min="98" max="98" width="6" bestFit="1" customWidth="1"/>
     <col min="99" max="99" width="3" bestFit="1" customWidth="1"/>
-    <col min="100" max="100" width="6.42578125" bestFit="1" customWidth="1"/>
+    <col min="100" max="100" width="6.5" bestFit="1" customWidth="1"/>
     <col min="101" max="101" width="6" bestFit="1" customWidth="1"/>
-    <col min="102" max="102" width="6.42578125" bestFit="1" customWidth="1"/>
+    <col min="102" max="102" width="6.5" bestFit="1" customWidth="1"/>
     <col min="103" max="103" width="6" bestFit="1" customWidth="1"/>
-    <col min="104" max="104" width="6.42578125" bestFit="1" customWidth="1"/>
+    <col min="104" max="104" width="6.5" bestFit="1" customWidth="1"/>
     <col min="105" max="105" width="6" bestFit="1" customWidth="1"/>
-    <col min="106" max="106" width="6.5703125" bestFit="1" customWidth="1"/>
+    <col min="106" max="106" width="6.5" bestFit="1" customWidth="1"/>
     <col min="107" max="107" width="6" bestFit="1" customWidth="1"/>
-    <col min="108" max="108" width="6.5703125" bestFit="1" customWidth="1"/>
+    <col min="108" max="108" width="6.5" bestFit="1" customWidth="1"/>
     <col min="109" max="109" width="6" bestFit="1" customWidth="1"/>
-    <col min="110" max="110" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="110" max="110" width="7.5" bestFit="1" customWidth="1"/>
     <col min="111" max="111" width="6" bestFit="1" customWidth="1"/>
-    <col min="112" max="112" width="5.85546875" bestFit="1" customWidth="1"/>
+    <col min="112" max="112" width="5.83203125" bestFit="1" customWidth="1"/>
     <col min="113" max="113" width="6" bestFit="1" customWidth="1"/>
     <col min="114" max="114" width="15" bestFit="1" customWidth="1"/>
     <col min="115" max="117" width="6" bestFit="1" customWidth="1"/>
-    <col min="118" max="118" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="118" max="118" width="10.5" bestFit="1" customWidth="1"/>
     <col min="119" max="119" width="6" bestFit="1" customWidth="1"/>
-    <col min="120" max="120" width="6.42578125" bestFit="1" customWidth="1"/>
-    <col min="121" max="121" width="5.28515625" bestFit="1" customWidth="1"/>
-    <col min="122" max="122" width="2.140625" bestFit="1" customWidth="1"/>
-    <col min="123" max="123" width="6.42578125" bestFit="1" customWidth="1"/>
-    <col min="124" max="124" width="5.28515625" bestFit="1" customWidth="1"/>
-    <col min="125" max="125" width="2.140625" bestFit="1" customWidth="1"/>
-    <col min="126" max="126" width="6.42578125" bestFit="1" customWidth="1"/>
-    <col min="127" max="127" width="5.28515625" bestFit="1" customWidth="1"/>
-    <col min="128" max="128" width="2.140625" bestFit="1" customWidth="1"/>
-    <col min="129" max="129" width="6.5703125" bestFit="1" customWidth="1"/>
-    <col min="130" max="130" width="5.28515625" bestFit="1" customWidth="1"/>
-    <col min="131" max="131" width="2.140625" bestFit="1" customWidth="1"/>
-    <col min="132" max="132" width="6.5703125" bestFit="1" customWidth="1"/>
-    <col min="133" max="133" width="5.28515625" bestFit="1" customWidth="1"/>
-    <col min="134" max="134" width="2.140625" bestFit="1" customWidth="1"/>
-    <col min="135" max="135" width="7.5703125" bestFit="1" customWidth="1"/>
-    <col min="136" max="136" width="5.28515625" bestFit="1" customWidth="1"/>
-    <col min="137" max="137" width="2.140625" bestFit="1" customWidth="1"/>
-    <col min="138" max="138" width="5.85546875" bestFit="1" customWidth="1"/>
-    <col min="139" max="139" width="5.28515625" bestFit="1" customWidth="1"/>
-    <col min="140" max="140" width="2.140625" bestFit="1" customWidth="1"/>
+    <col min="120" max="120" width="6.5" bestFit="1" customWidth="1"/>
+    <col min="121" max="121" width="5.33203125" bestFit="1" customWidth="1"/>
+    <col min="122" max="122" width="2.1640625" bestFit="1" customWidth="1"/>
+    <col min="123" max="123" width="6.5" bestFit="1" customWidth="1"/>
+    <col min="124" max="124" width="5.33203125" bestFit="1" customWidth="1"/>
+    <col min="125" max="125" width="2.1640625" bestFit="1" customWidth="1"/>
+    <col min="126" max="126" width="6.5" bestFit="1" customWidth="1"/>
+    <col min="127" max="127" width="5.33203125" bestFit="1" customWidth="1"/>
+    <col min="128" max="128" width="2.1640625" bestFit="1" customWidth="1"/>
+    <col min="129" max="129" width="6.5" bestFit="1" customWidth="1"/>
+    <col min="130" max="130" width="5.33203125" bestFit="1" customWidth="1"/>
+    <col min="131" max="131" width="2.1640625" bestFit="1" customWidth="1"/>
+    <col min="132" max="132" width="6.5" bestFit="1" customWidth="1"/>
+    <col min="133" max="133" width="5.33203125" bestFit="1" customWidth="1"/>
+    <col min="134" max="134" width="2.1640625" bestFit="1" customWidth="1"/>
+    <col min="135" max="135" width="7.5" bestFit="1" customWidth="1"/>
+    <col min="136" max="136" width="5.33203125" bestFit="1" customWidth="1"/>
+    <col min="137" max="137" width="2.1640625" bestFit="1" customWidth="1"/>
+    <col min="138" max="138" width="5.83203125" bestFit="1" customWidth="1"/>
+    <col min="139" max="139" width="5.33203125" bestFit="1" customWidth="1"/>
+    <col min="140" max="140" width="2.1640625" bestFit="1" customWidth="1"/>
     <col min="141" max="141" width="6" bestFit="1" customWidth="1"/>
-    <col min="142" max="142" width="5.28515625" bestFit="1" customWidth="1"/>
-    <col min="143" max="143" width="2.140625" bestFit="1" customWidth="1"/>
-    <col min="144" max="145" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="146" max="146" width="2.7109375" bestFit="1" customWidth="1"/>
-    <col min="147" max="147" width="2.28515625" bestFit="1" customWidth="1"/>
-    <col min="148" max="148" width="5.5703125" bestFit="1" customWidth="1"/>
-    <col min="149" max="149" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="150" max="150" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="151" max="151" width="2.7109375" bestFit="1" customWidth="1"/>
-    <col min="152" max="152" width="2.28515625" bestFit="1" customWidth="1"/>
-    <col min="153" max="153" width="5.5703125" bestFit="1" customWidth="1"/>
-    <col min="154" max="154" width="3.85546875" bestFit="1" customWidth="1"/>
-    <col min="155" max="155" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="156" max="156" width="2.7109375" bestFit="1" customWidth="1"/>
-    <col min="157" max="157" width="2.28515625" bestFit="1" customWidth="1"/>
-    <col min="158" max="158" width="5.5703125" bestFit="1" customWidth="1"/>
-    <col min="159" max="159" width="6.140625" bestFit="1" customWidth="1"/>
-    <col min="160" max="160" width="2.7109375" bestFit="1" customWidth="1"/>
-    <col min="161" max="161" width="2.28515625" bestFit="1" customWidth="1"/>
-    <col min="162" max="162" width="5.5703125" bestFit="1" customWidth="1"/>
-    <col min="163" max="163" width="6.42578125" bestFit="1" customWidth="1"/>
-    <col min="164" max="164" width="2.7109375" bestFit="1" customWidth="1"/>
-    <col min="165" max="165" width="2.28515625" bestFit="1" customWidth="1"/>
-    <col min="166" max="166" width="5.5703125" bestFit="1" customWidth="1"/>
-    <col min="167" max="167" width="7.42578125" bestFit="1" customWidth="1"/>
-    <col min="168" max="168" width="2.7109375" bestFit="1" customWidth="1"/>
-    <col min="169" max="169" width="2.28515625" bestFit="1" customWidth="1"/>
-    <col min="170" max="170" width="5.5703125" bestFit="1" customWidth="1"/>
-    <col min="171" max="171" width="5.85546875" bestFit="1" customWidth="1"/>
-    <col min="172" max="172" width="2.7109375" bestFit="1" customWidth="1"/>
-    <col min="173" max="173" width="2.28515625" bestFit="1" customWidth="1"/>
-    <col min="174" max="174" width="5.5703125" bestFit="1" customWidth="1"/>
+    <col min="142" max="142" width="5.33203125" bestFit="1" customWidth="1"/>
+    <col min="143" max="143" width="2.1640625" bestFit="1" customWidth="1"/>
+    <col min="144" max="145" width="8.5" bestFit="1" customWidth="1"/>
+    <col min="146" max="146" width="2.6640625" bestFit="1" customWidth="1"/>
+    <col min="147" max="147" width="2.33203125" bestFit="1" customWidth="1"/>
+    <col min="148" max="148" width="5.5" bestFit="1" customWidth="1"/>
+    <col min="149" max="149" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="150" max="150" width="8.5" bestFit="1" customWidth="1"/>
+    <col min="151" max="151" width="2.6640625" bestFit="1" customWidth="1"/>
+    <col min="152" max="152" width="2.33203125" bestFit="1" customWidth="1"/>
+    <col min="153" max="153" width="5.5" bestFit="1" customWidth="1"/>
+    <col min="154" max="154" width="3.83203125" bestFit="1" customWidth="1"/>
+    <col min="155" max="155" width="8.5" bestFit="1" customWidth="1"/>
+    <col min="156" max="156" width="2.6640625" bestFit="1" customWidth="1"/>
+    <col min="157" max="157" width="2.33203125" bestFit="1" customWidth="1"/>
+    <col min="158" max="158" width="5.5" bestFit="1" customWidth="1"/>
+    <col min="159" max="159" width="6.1640625" bestFit="1" customWidth="1"/>
+    <col min="160" max="160" width="2.6640625" bestFit="1" customWidth="1"/>
+    <col min="161" max="161" width="2.33203125" bestFit="1" customWidth="1"/>
+    <col min="162" max="162" width="5.5" bestFit="1" customWidth="1"/>
+    <col min="163" max="163" width="6.5" bestFit="1" customWidth="1"/>
+    <col min="164" max="164" width="2.6640625" bestFit="1" customWidth="1"/>
+    <col min="165" max="165" width="2.33203125" bestFit="1" customWidth="1"/>
+    <col min="166" max="166" width="5.5" bestFit="1" customWidth="1"/>
+    <col min="167" max="167" width="7.5" bestFit="1" customWidth="1"/>
+    <col min="168" max="168" width="2.6640625" bestFit="1" customWidth="1"/>
+    <col min="169" max="169" width="2.33203125" bestFit="1" customWidth="1"/>
+    <col min="170" max="170" width="5.5" bestFit="1" customWidth="1"/>
+    <col min="171" max="171" width="5.83203125" bestFit="1" customWidth="1"/>
+    <col min="172" max="172" width="2.6640625" bestFit="1" customWidth="1"/>
+    <col min="173" max="173" width="2.33203125" bestFit="1" customWidth="1"/>
+    <col min="174" max="174" width="5.5" bestFit="1" customWidth="1"/>
     <col min="175" max="175" width="6" bestFit="1" customWidth="1"/>
-    <col min="176" max="176" width="2.7109375" bestFit="1" customWidth="1"/>
-    <col min="177" max="177" width="2.28515625" bestFit="1" customWidth="1"/>
-    <col min="178" max="178" width="5.5703125" bestFit="1" customWidth="1"/>
-    <col min="179" max="179" width="7.5703125" bestFit="1" customWidth="1"/>
-    <col min="180" max="180" width="2.7109375" bestFit="1" customWidth="1"/>
-    <col min="181" max="181" width="2.28515625" bestFit="1" customWidth="1"/>
-    <col min="182" max="182" width="5.5703125" bestFit="1" customWidth="1"/>
+    <col min="176" max="176" width="2.6640625" bestFit="1" customWidth="1"/>
+    <col min="177" max="177" width="2.33203125" bestFit="1" customWidth="1"/>
+    <col min="178" max="178" width="5.5" bestFit="1" customWidth="1"/>
+    <col min="179" max="179" width="7.5" bestFit="1" customWidth="1"/>
+    <col min="180" max="180" width="2.6640625" bestFit="1" customWidth="1"/>
+    <col min="181" max="181" width="2.33203125" bestFit="1" customWidth="1"/>
+    <col min="182" max="182" width="5.5" bestFit="1" customWidth="1"/>
     <col min="183" max="183" width="5" bestFit="1" customWidth="1"/>
-    <col min="184" max="184" width="2.7109375" bestFit="1" customWidth="1"/>
-    <col min="185" max="185" width="3.5703125" bestFit="1" customWidth="1"/>
-    <col min="186" max="186" width="5.7109375" bestFit="1" customWidth="1"/>
-    <col min="187" max="187" width="2.7109375" bestFit="1" customWidth="1"/>
-    <col min="188" max="188" width="3.5703125" bestFit="1" customWidth="1"/>
-    <col min="189" max="189" width="6.42578125" bestFit="1" customWidth="1"/>
-    <col min="190" max="190" width="2.7109375" bestFit="1" customWidth="1"/>
-    <col min="191" max="191" width="5.7109375" bestFit="1" customWidth="1"/>
-    <col min="192" max="192" width="3.5703125" bestFit="1" customWidth="1"/>
+    <col min="184" max="184" width="2.6640625" bestFit="1" customWidth="1"/>
+    <col min="185" max="185" width="3.5" bestFit="1" customWidth="1"/>
+    <col min="186" max="186" width="5.6640625" bestFit="1" customWidth="1"/>
+    <col min="187" max="187" width="2.6640625" bestFit="1" customWidth="1"/>
+    <col min="188" max="188" width="3.5" bestFit="1" customWidth="1"/>
+    <col min="189" max="189" width="6.5" bestFit="1" customWidth="1"/>
+    <col min="190" max="190" width="2.6640625" bestFit="1" customWidth="1"/>
+    <col min="191" max="191" width="5.6640625" bestFit="1" customWidth="1"/>
+    <col min="192" max="192" width="3.5" bestFit="1" customWidth="1"/>
     <col min="193" max="193" width="6" bestFit="1" customWidth="1"/>
-    <col min="194" max="194" width="2.7109375" bestFit="1" customWidth="1"/>
-    <col min="195" max="195" width="3.5703125" bestFit="1" customWidth="1"/>
-    <col min="196" max="196" width="5.85546875" bestFit="1" customWidth="1"/>
-    <col min="197" max="197" width="2.7109375" bestFit="1" customWidth="1"/>
-    <col min="198" max="198" width="5.7109375" bestFit="1" customWidth="1"/>
-    <col min="199" max="199" width="3.5703125" bestFit="1" customWidth="1"/>
-    <col min="200" max="200" width="4.140625" bestFit="1" customWidth="1"/>
-    <col min="201" max="201" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="194" max="194" width="2.6640625" bestFit="1" customWidth="1"/>
+    <col min="195" max="195" width="3.5" bestFit="1" customWidth="1"/>
+    <col min="196" max="196" width="5.83203125" bestFit="1" customWidth="1"/>
+    <col min="197" max="197" width="2.6640625" bestFit="1" customWidth="1"/>
+    <col min="198" max="198" width="5.6640625" bestFit="1" customWidth="1"/>
+    <col min="199" max="199" width="3.5" bestFit="1" customWidth="1"/>
+    <col min="200" max="200" width="4.1640625" bestFit="1" customWidth="1"/>
+    <col min="201" max="201" width="7.5" bestFit="1" customWidth="1"/>
     <col min="202" max="202" width="11" bestFit="1" customWidth="1"/>
-    <col min="203" max="203" width="4.140625" bestFit="1" customWidth="1"/>
-    <col min="204" max="204" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="203" max="203" width="4.1640625" bestFit="1" customWidth="1"/>
+    <col min="204" max="204" width="7.5" bestFit="1" customWidth="1"/>
     <col min="205" max="205" width="11" bestFit="1" customWidth="1"/>
-    <col min="206" max="206" width="5.7109375" bestFit="1" customWidth="1"/>
+    <col min="206" max="206" width="5.6640625" bestFit="1" customWidth="1"/>
     <col min="207" max="207" width="11" bestFit="1" customWidth="1"/>
-    <col min="208" max="208" width="7.5703125" bestFit="1" customWidth="1"/>
-    <col min="209" max="209" width="4.5703125" bestFit="1" customWidth="1"/>
+    <col min="208" max="208" width="7.5" bestFit="1" customWidth="1"/>
+    <col min="209" max="209" width="4.5" bestFit="1" customWidth="1"/>
     <col min="210" max="210" width="11" bestFit="1" customWidth="1"/>
-    <col min="211" max="211" width="6.42578125" bestFit="1" customWidth="1"/>
-    <col min="212" max="212" width="4.5703125" bestFit="1" customWidth="1"/>
+    <col min="211" max="211" width="6.5" bestFit="1" customWidth="1"/>
+    <col min="212" max="212" width="4.5" bestFit="1" customWidth="1"/>
     <col min="213" max="213" width="11" bestFit="1" customWidth="1"/>
-    <col min="214" max="214" width="4.5703125" bestFit="1" customWidth="1"/>
+    <col min="214" max="214" width="4.5" bestFit="1" customWidth="1"/>
     <col min="215" max="215" width="7" bestFit="1" customWidth="1"/>
-    <col min="216" max="216" width="4.5703125" bestFit="1" customWidth="1"/>
+    <col min="216" max="216" width="4.5" bestFit="1" customWidth="1"/>
     <col min="217" max="217" width="7" bestFit="1" customWidth="1"/>
-    <col min="218" max="218" width="4.5703125" bestFit="1" customWidth="1"/>
+    <col min="218" max="218" width="4.5" bestFit="1" customWidth="1"/>
     <col min="219" max="219" width="7" bestFit="1" customWidth="1"/>
-    <col min="220" max="220" width="3.85546875" bestFit="1" customWidth="1"/>
-    <col min="221" max="221" width="2.140625" bestFit="1" customWidth="1"/>
+    <col min="220" max="220" width="3.83203125" bestFit="1" customWidth="1"/>
+    <col min="221" max="221" width="2.1640625" bestFit="1" customWidth="1"/>
     <col min="222" max="222" width="7" bestFit="1" customWidth="1"/>
-    <col min="223" max="223" width="2.28515625" bestFit="1" customWidth="1"/>
+    <col min="223" max="223" width="2.33203125" bestFit="1" customWidth="1"/>
     <col min="224" max="224" width="7" bestFit="1" customWidth="1"/>
-    <col min="225" max="225" width="3.5703125" bestFit="1" customWidth="1"/>
+    <col min="225" max="225" width="3.5" bestFit="1" customWidth="1"/>
     <col min="226" max="226" width="7" bestFit="1" customWidth="1"/>
-    <col min="227" max="227" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="227" max="227" width="8.5" bestFit="1" customWidth="1"/>
     <col min="228" max="228" width="7" bestFit="1" customWidth="1"/>
     <col min="229" max="229" width="5" bestFit="1" customWidth="1"/>
     <col min="230" max="230" width="7" bestFit="1" customWidth="1"/>
-    <col min="231" max="231" width="4.85546875" bestFit="1" customWidth="1"/>
-    <col min="232" max="232" width="6.42578125" bestFit="1" customWidth="1"/>
-    <col min="233" max="233" width="2.28515625" bestFit="1" customWidth="1"/>
-    <col min="234" max="234" width="5.5703125" bestFit="1" customWidth="1"/>
-    <col min="235" max="235" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="236" max="236" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="237" max="237" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="238" max="238" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="239" max="239" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="240" max="240" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="241" max="241" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="242" max="242" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="243" max="244" width="6.5703125" bestFit="1" customWidth="1"/>
-    <col min="245" max="245" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="246" max="246" width="6.42578125" bestFit="1" customWidth="1"/>
-    <col min="247" max="250" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="251" max="252" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="231" max="231" width="4.83203125" bestFit="1" customWidth="1"/>
+    <col min="232" max="232" width="6.5" bestFit="1" customWidth="1"/>
+    <col min="233" max="233" width="2.33203125" bestFit="1" customWidth="1"/>
+    <col min="234" max="234" width="5.5" bestFit="1" customWidth="1"/>
+    <col min="235" max="235" width="19.5" bestFit="1" customWidth="1"/>
+    <col min="236" max="236" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="237" max="237" width="19.5" bestFit="1" customWidth="1"/>
+    <col min="238" max="238" width="17.5" bestFit="1" customWidth="1"/>
+    <col min="239" max="239" width="10.83203125" bestFit="1" customWidth="1"/>
+    <col min="240" max="240" width="9.83203125" bestFit="1" customWidth="1"/>
+    <col min="241" max="241" width="8.5" bestFit="1" customWidth="1"/>
+    <col min="242" max="242" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="243" max="244" width="6.5" bestFit="1" customWidth="1"/>
+    <col min="245" max="245" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="246" max="246" width="6.5" bestFit="1" customWidth="1"/>
+    <col min="247" max="250" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="251" max="252" width="8.5" bestFit="1" customWidth="1"/>
     <col min="253" max="254" width="18" bestFit="1" customWidth="1"/>
-    <col min="255" max="255" width="6.7109375" bestFit="1" customWidth="1"/>
-    <col min="256" max="256" width="26.5703125" bestFit="1" customWidth="1"/>
-    <col min="257" max="258" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="259" max="259" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="255" max="255" width="6.6640625" bestFit="1" customWidth="1"/>
+    <col min="256" max="256" width="26.5" bestFit="1" customWidth="1"/>
+    <col min="257" max="258" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="259" max="259" width="16.6640625" bestFit="1" customWidth="1"/>
     <col min="260" max="260" width="18" bestFit="1" customWidth="1"/>
-    <col min="261" max="262" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="261" max="262" width="9.5" bestFit="1" customWidth="1"/>
     <col min="263" max="263" width="6" bestFit="1" customWidth="1"/>
-    <col min="264" max="264" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="264" max="264" width="9.5" bestFit="1" customWidth="1"/>
     <col min="265" max="265" width="18" bestFit="1" customWidth="1"/>
-    <col min="266" max="266" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="267" max="268" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="266" max="266" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="267" max="268" width="7.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" s="6" t="s">
         <v>132</v>
       </c>
@@ -3128,7 +3125,7 @@
         <v>555</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>110</v>
       </c>
@@ -3157,7 +3154,7 @@
         <v>556</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>108</v>
       </c>
@@ -3186,7 +3183,7 @@
         <v>557</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>92</v>
       </c>
@@ -3215,7 +3212,7 @@
         <v>558</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>114</v>
       </c>
@@ -3244,7 +3241,7 @@
         <v>559</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>52</v>
       </c>
@@ -3273,7 +3270,7 @@
         <v>560</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>55</v>
       </c>
@@ -3302,7 +3299,7 @@
         <v>561</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>119</v>
       </c>
@@ -3328,7 +3325,7 @@
         <v>562</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>90</v>
       </c>
@@ -3357,7 +3354,7 @@
         <v>563</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>112</v>
       </c>
@@ -3386,7 +3383,7 @@
         <v>564</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>61</v>
       </c>
@@ -3415,7 +3412,7 @@
         <v>565</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>65</v>
       </c>
@@ -3444,7 +3441,7 @@
         <v>566</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>75</v>
       </c>
@@ -3473,7 +3470,7 @@
         <v>567</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>67</v>
       </c>
@@ -3502,7 +3499,7 @@
         <v>568</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>78</v>
       </c>
@@ -3531,7 +3528,7 @@
         <v>569</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>94</v>
       </c>
@@ -3560,7 +3557,7 @@
         <v>570</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>86</v>
       </c>
@@ -3589,7 +3586,7 @@
         <v>571</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>117</v>
       </c>
@@ -3618,7 +3615,7 @@
         <v>572</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>38</v>
       </c>
@@ -3647,7 +3644,7 @@
         <v>573</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>40</v>
       </c>
@@ -3676,7 +3673,7 @@
         <v>574</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>36</v>
       </c>
@@ -3705,7 +3702,7 @@
         <v>575</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>28</v>
       </c>
@@ -3734,7 +3731,7 @@
         <v>576</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>96</v>
       </c>
@@ -3763,7 +3760,7 @@
         <v>577</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>11</v>
       </c>
@@ -3792,7 +3789,7 @@
         <v>578</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>9</v>
       </c>
@@ -3821,7 +3818,7 @@
         <v>579</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>98</v>
       </c>
@@ -3850,7 +3847,7 @@
         <v>580</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>129</v>
       </c>
@@ -3876,7 +3873,7 @@
         <v>581</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>125</v>
       </c>
@@ -3902,7 +3899,7 @@
         <v>582</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>63</v>
       </c>
@@ -3931,7 +3928,7 @@
         <v>583</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>88</v>
       </c>
@@ -3960,7 +3957,7 @@
         <v>584</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>34</v>
       </c>
@@ -3989,7 +3986,7 @@
         <v>585</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>26</v>
       </c>
@@ -4018,7 +4015,7 @@
         <v>586</v>
       </c>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>100</v>
       </c>
@@ -4047,7 +4044,7 @@
         <v>587</v>
       </c>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>13</v>
       </c>
@@ -4076,7 +4073,7 @@
         <v>588</v>
       </c>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>17</v>
       </c>
@@ -4105,7 +4102,7 @@
         <v>589</v>
       </c>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>15</v>
       </c>
@@ -4134,7 +4131,7 @@
         <v>590</v>
       </c>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>71</v>
       </c>
@@ -4163,7 +4160,7 @@
         <v>591</v>
       </c>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>82</v>
       </c>
@@ -4192,7 +4189,7 @@
         <v>592</v>
       </c>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>2</v>
       </c>
@@ -4221,7 +4218,7 @@
         <v>593</v>
       </c>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>46</v>
       </c>
@@ -4250,7 +4247,7 @@
         <v>594</v>
       </c>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>104</v>
       </c>
@@ -4279,7 +4276,7 @@
         <v>595</v>
       </c>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>69</v>
       </c>
@@ -4308,7 +4305,7 @@
         <v>596</v>
       </c>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>80</v>
       </c>
@@ -4337,7 +4334,7 @@
         <v>597</v>
       </c>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>30</v>
       </c>
@@ -4366,7 +4363,7 @@
         <v>598</v>
       </c>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>42</v>
       </c>
@@ -4395,7 +4392,7 @@
         <v>599</v>
       </c>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>73</v>
       </c>
@@ -4424,7 +4421,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>84</v>
       </c>
@@ -4453,7 +4450,7 @@
         <v>601</v>
       </c>
     </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>19</v>
       </c>
@@ -4482,7 +4479,7 @@
         <v>602</v>
       </c>
     </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>21</v>
       </c>
@@ -4511,7 +4508,7 @@
         <v>603</v>
       </c>
     </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>48</v>
       </c>
@@ -4537,7 +4534,7 @@
         <v>604</v>
       </c>
     </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>5</v>
       </c>
@@ -4563,7 +4560,7 @@
         <v>605</v>
       </c>
     </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>50</v>
       </c>
@@ -4589,7 +4586,7 @@
         <v>606</v>
       </c>
     </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>57</v>
       </c>
@@ -4615,7 +4612,7 @@
         <v>607</v>
       </c>
     </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>44</v>
       </c>
@@ -4638,7 +4635,7 @@
         <v>608</v>
       </c>
     </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>106</v>
       </c>
@@ -4661,7 +4658,7 @@
         <v>609</v>
       </c>
     </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>59</v>
       </c>
@@ -4681,7 +4678,7 @@
         <v>610</v>
       </c>
     </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>102</v>
       </c>
@@ -4704,7 +4701,7 @@
         <v>611</v>
       </c>
     </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>32</v>
       </c>
@@ -4727,7 +4724,7 @@
         <v>612</v>
       </c>
     </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>23</v>
       </c>
@@ -4750,7 +4747,7 @@
         <v>613</v>
       </c>
     </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>127</v>
       </c>
@@ -4770,7 +4767,7 @@
         <v>614</v>
       </c>
     </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>123</v>
       </c>
@@ -4790,7 +4787,7 @@
         <v>615</v>
       </c>
     </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>7</v>
       </c>
@@ -4813,7 +4810,7 @@
         <v>616</v>
       </c>
     </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>121</v>
       </c>
@@ -4833,7 +4830,7 @@
         <v>617</v>
       </c>
     </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:11" x14ac:dyDescent="0.2">
       <c r="H64" t="s">
         <v>349</v>
       </c>
@@ -4841,7 +4838,7 @@
         <v>618</v>
       </c>
     </row>
-    <row r="65" spans="8:11" x14ac:dyDescent="0.25">
+    <row r="65" spans="8:11" x14ac:dyDescent="0.2">
       <c r="H65" t="s">
         <v>350</v>
       </c>
@@ -4849,7 +4846,7 @@
         <v>619</v>
       </c>
     </row>
-    <row r="66" spans="8:11" x14ac:dyDescent="0.25">
+    <row r="66" spans="8:11" x14ac:dyDescent="0.2">
       <c r="H66" t="s">
         <v>351</v>
       </c>
@@ -4857,7 +4854,7 @@
         <v>620</v>
       </c>
     </row>
-    <row r="67" spans="8:11" x14ac:dyDescent="0.25">
+    <row r="67" spans="8:11" x14ac:dyDescent="0.2">
       <c r="H67" t="s">
         <v>352</v>
       </c>
@@ -4865,7 +4862,7 @@
         <v>621</v>
       </c>
     </row>
-    <row r="68" spans="8:11" x14ac:dyDescent="0.25">
+    <row r="68" spans="8:11" x14ac:dyDescent="0.2">
       <c r="H68" t="s">
         <v>353</v>
       </c>
@@ -4873,7 +4870,7 @@
         <v>622</v>
       </c>
     </row>
-    <row r="69" spans="8:11" x14ac:dyDescent="0.25">
+    <row r="69" spans="8:11" x14ac:dyDescent="0.2">
       <c r="H69" t="s">
         <v>354</v>
       </c>
@@ -4881,7 +4878,7 @@
         <v>623</v>
       </c>
     </row>
-    <row r="70" spans="8:11" x14ac:dyDescent="0.25">
+    <row r="70" spans="8:11" x14ac:dyDescent="0.2">
       <c r="H70" t="s">
         <v>355</v>
       </c>
@@ -4889,7 +4886,7 @@
         <v>624</v>
       </c>
     </row>
-    <row r="71" spans="8:11" x14ac:dyDescent="0.25">
+    <row r="71" spans="8:11" x14ac:dyDescent="0.2">
       <c r="H71" t="s">
         <v>356</v>
       </c>
@@ -4897,7 +4894,7 @@
         <v>625</v>
       </c>
     </row>
-    <row r="72" spans="8:11" x14ac:dyDescent="0.25">
+    <row r="72" spans="8:11" x14ac:dyDescent="0.2">
       <c r="H72" t="s">
         <v>357</v>
       </c>
@@ -4905,7 +4902,7 @@
         <v>626</v>
       </c>
     </row>
-    <row r="73" spans="8:11" x14ac:dyDescent="0.25">
+    <row r="73" spans="8:11" x14ac:dyDescent="0.2">
       <c r="H73" t="s">
         <v>359</v>
       </c>
@@ -4913,7 +4910,7 @@
         <v>627</v>
       </c>
     </row>
-    <row r="74" spans="8:11" x14ac:dyDescent="0.25">
+    <row r="74" spans="8:11" x14ac:dyDescent="0.2">
       <c r="H74" t="s">
         <v>360</v>
       </c>
@@ -4921,7 +4918,7 @@
         <v>628</v>
       </c>
     </row>
-    <row r="75" spans="8:11" x14ac:dyDescent="0.25">
+    <row r="75" spans="8:11" x14ac:dyDescent="0.2">
       <c r="H75" t="s">
         <v>361</v>
       </c>
@@ -4929,7 +4926,7 @@
         <v>629</v>
       </c>
     </row>
-    <row r="76" spans="8:11" x14ac:dyDescent="0.25">
+    <row r="76" spans="8:11" x14ac:dyDescent="0.2">
       <c r="H76" t="s">
         <v>362</v>
       </c>
@@ -4937,7 +4934,7 @@
         <v>630</v>
       </c>
     </row>
-    <row r="77" spans="8:11" x14ac:dyDescent="0.25">
+    <row r="77" spans="8:11" x14ac:dyDescent="0.2">
       <c r="H77" t="s">
         <v>363</v>
       </c>
@@ -4945,7 +4942,7 @@
         <v>631</v>
       </c>
     </row>
-    <row r="78" spans="8:11" x14ac:dyDescent="0.25">
+    <row r="78" spans="8:11" x14ac:dyDescent="0.2">
       <c r="H78" t="s">
         <v>364</v>
       </c>
@@ -4953,912 +4950,912 @@
         <v>632</v>
       </c>
     </row>
-    <row r="79" spans="8:11" x14ac:dyDescent="0.25">
+    <row r="79" spans="8:11" x14ac:dyDescent="0.2">
       <c r="H79" t="s">
         <v>365</v>
       </c>
     </row>
-    <row r="80" spans="8:11" x14ac:dyDescent="0.25">
+    <row r="80" spans="8:11" x14ac:dyDescent="0.2">
       <c r="H80" t="s">
         <v>366</v>
       </c>
     </row>
-    <row r="81" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="81" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H81" t="s">
         <v>367</v>
       </c>
     </row>
-    <row r="82" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="82" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H82" t="s">
         <v>368</v>
       </c>
     </row>
-    <row r="83" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="83" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H83" t="s">
         <v>369</v>
       </c>
     </row>
-    <row r="84" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="84" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H84" t="s">
         <v>371</v>
       </c>
     </row>
-    <row r="85" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="85" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H85" t="s">
         <v>372</v>
       </c>
     </row>
-    <row r="86" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="86" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H86" t="s">
         <v>373</v>
       </c>
     </row>
-    <row r="87" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="87" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H87" t="s">
         <v>374</v>
       </c>
     </row>
-    <row r="88" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="88" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H88" t="s">
         <v>375</v>
       </c>
     </row>
-    <row r="89" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="89" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H89" t="s">
         <v>376</v>
       </c>
     </row>
-    <row r="90" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="90" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H90" t="s">
         <v>377</v>
       </c>
     </row>
-    <row r="91" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="91" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H91" t="s">
         <v>380</v>
       </c>
     </row>
-    <row r="92" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="92" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H92" t="s">
         <v>381</v>
       </c>
     </row>
-    <row r="93" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="93" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H93" t="s">
         <v>382</v>
       </c>
     </row>
-    <row r="94" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="94" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H94" t="s">
         <v>384</v>
       </c>
     </row>
-    <row r="95" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="95" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H95" t="s">
         <v>385</v>
       </c>
     </row>
-    <row r="96" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="96" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H96" t="s">
         <v>386</v>
       </c>
     </row>
-    <row r="97" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="97" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H97" t="s">
         <v>387</v>
       </c>
     </row>
-    <row r="98" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="98" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H98" t="s">
         <v>388</v>
       </c>
     </row>
-    <row r="99" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="99" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H99" t="s">
         <v>389</v>
       </c>
     </row>
-    <row r="100" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="100" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H100" t="s">
         <v>390</v>
       </c>
     </row>
-    <row r="101" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="101" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H101" t="s">
         <v>391</v>
       </c>
     </row>
-    <row r="102" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="102" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H102" t="s">
         <v>393</v>
       </c>
     </row>
-    <row r="103" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="103" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H103" t="s">
         <v>394</v>
       </c>
     </row>
-    <row r="104" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="104" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H104" t="s">
         <v>395</v>
       </c>
     </row>
-    <row r="105" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="105" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H105" t="s">
         <v>396</v>
       </c>
     </row>
-    <row r="106" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="106" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H106" t="s">
         <v>397</v>
       </c>
     </row>
-    <row r="107" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="107" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H107" t="s">
         <v>398</v>
       </c>
     </row>
-    <row r="108" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="108" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H108" t="s">
         <v>399</v>
       </c>
     </row>
-    <row r="109" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="109" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H109" t="s">
         <v>400</v>
       </c>
     </row>
-    <row r="110" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="110" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H110" t="s">
         <v>401</v>
       </c>
     </row>
-    <row r="111" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="111" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H111" t="s">
         <v>402</v>
       </c>
     </row>
-    <row r="112" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="112" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H112" t="s">
         <v>403</v>
       </c>
     </row>
-    <row r="113" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="113" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H113" t="s">
         <v>404</v>
       </c>
     </row>
-    <row r="114" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="114" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H114" t="s">
         <v>405</v>
       </c>
     </row>
-    <row r="115" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="115" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H115" t="s">
         <v>406</v>
       </c>
     </row>
-    <row r="116" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="116" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H116" t="s">
         <v>407</v>
       </c>
     </row>
-    <row r="117" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="117" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H117" t="s">
         <v>408</v>
       </c>
     </row>
-    <row r="118" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="118" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H118" t="s">
         <v>409</v>
       </c>
     </row>
-    <row r="119" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="119" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H119" t="s">
         <v>410</v>
       </c>
     </row>
-    <row r="120" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="120" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H120" t="s">
         <v>411</v>
       </c>
     </row>
-    <row r="121" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="121" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H121" t="s">
         <v>412</v>
       </c>
     </row>
-    <row r="122" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="122" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H122" t="s">
         <v>413</v>
       </c>
     </row>
-    <row r="123" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="123" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H123" t="s">
         <v>414</v>
       </c>
     </row>
-    <row r="124" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="124" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H124" t="s">
         <v>415</v>
       </c>
     </row>
-    <row r="125" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="125" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H125" t="s">
         <v>416</v>
       </c>
     </row>
-    <row r="126" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="126" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H126" t="s">
         <v>417</v>
       </c>
     </row>
-    <row r="127" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="127" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H127" t="s">
         <v>418</v>
       </c>
     </row>
-    <row r="128" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="128" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H128" t="s">
         <v>419</v>
       </c>
     </row>
-    <row r="129" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="129" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H129" t="s">
         <v>420</v>
       </c>
     </row>
-    <row r="130" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="130" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H130" t="s">
         <v>421</v>
       </c>
     </row>
-    <row r="131" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="131" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H131" t="s">
         <v>422</v>
       </c>
     </row>
-    <row r="132" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="132" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H132" t="s">
         <v>423</v>
       </c>
     </row>
-    <row r="133" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="133" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H133" t="s">
         <v>424</v>
       </c>
     </row>
-    <row r="134" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="134" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H134" t="s">
         <v>425</v>
       </c>
     </row>
-    <row r="135" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="135" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H135" t="s">
         <v>426</v>
       </c>
     </row>
-    <row r="136" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="136" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H136" t="s">
         <v>427</v>
       </c>
     </row>
-    <row r="137" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="137" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H137" t="s">
         <v>428</v>
       </c>
     </row>
-    <row r="138" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="138" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H138" t="s">
         <v>429</v>
       </c>
     </row>
-    <row r="139" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="139" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H139" t="s">
         <v>430</v>
       </c>
     </row>
-    <row r="140" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="140" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H140" t="s">
         <v>431</v>
       </c>
     </row>
-    <row r="141" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="141" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H141" t="s">
         <v>432</v>
       </c>
     </row>
-    <row r="142" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="142" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H142" t="s">
         <v>433</v>
       </c>
     </row>
-    <row r="143" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="143" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H143" t="s">
         <v>434</v>
       </c>
     </row>
-    <row r="144" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="144" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H144" t="s">
         <v>435</v>
       </c>
     </row>
-    <row r="145" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="145" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H145" t="s">
         <v>436</v>
       </c>
     </row>
-    <row r="146" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="146" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H146" t="s">
         <v>437</v>
       </c>
     </row>
-    <row r="147" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="147" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H147" t="s">
         <v>438</v>
       </c>
     </row>
-    <row r="148" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="148" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H148" t="s">
         <v>439</v>
       </c>
     </row>
-    <row r="149" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="149" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H149" t="s">
         <v>440</v>
       </c>
     </row>
-    <row r="150" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="150" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H150" t="s">
         <v>441</v>
       </c>
     </row>
-    <row r="151" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="151" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H151" t="s">
         <v>442</v>
       </c>
     </row>
-    <row r="152" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="152" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H152" t="s">
         <v>443</v>
       </c>
     </row>
-    <row r="153" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="153" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H153" t="s">
         <v>444</v>
       </c>
     </row>
-    <row r="154" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="154" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H154" t="s">
         <v>445</v>
       </c>
     </row>
-    <row r="155" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="155" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H155" t="s">
         <v>446</v>
       </c>
     </row>
-    <row r="156" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="156" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H156" t="s">
         <v>447</v>
       </c>
     </row>
-    <row r="157" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="157" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H157" t="s">
         <v>448</v>
       </c>
     </row>
-    <row r="158" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="158" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H158" t="s">
         <v>449</v>
       </c>
     </row>
-    <row r="159" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="159" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H159" t="s">
         <v>450</v>
       </c>
     </row>
-    <row r="160" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="160" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H160" t="s">
         <v>451</v>
       </c>
     </row>
-    <row r="161" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="161" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H161" t="s">
         <v>452</v>
       </c>
     </row>
-    <row r="162" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="162" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H162" t="s">
         <v>453</v>
       </c>
     </row>
-    <row r="163" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="163" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H163" t="s">
         <v>454</v>
       </c>
     </row>
-    <row r="164" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="164" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H164" t="s">
         <v>455</v>
       </c>
     </row>
-    <row r="165" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="165" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H165" t="s">
         <v>456</v>
       </c>
     </row>
-    <row r="166" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="166" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H166" t="s">
         <v>457</v>
       </c>
     </row>
-    <row r="167" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="167" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H167" t="s">
         <v>458</v>
       </c>
     </row>
-    <row r="168" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="168" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H168" t="s">
         <v>459</v>
       </c>
     </row>
-    <row r="169" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="169" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H169" t="s">
         <v>460</v>
       </c>
     </row>
-    <row r="170" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="170" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H170" t="s">
         <v>461</v>
       </c>
     </row>
-    <row r="171" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="171" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H171" t="s">
         <v>462</v>
       </c>
     </row>
-    <row r="172" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="172" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H172" t="s">
         <v>463</v>
       </c>
     </row>
-    <row r="173" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="173" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H173" t="s">
         <v>464</v>
       </c>
     </row>
-    <row r="174" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="174" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H174" t="s">
         <v>465</v>
       </c>
     </row>
-    <row r="175" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="175" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H175" t="s">
         <v>466</v>
       </c>
     </row>
-    <row r="176" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="176" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H176" t="s">
         <v>467</v>
       </c>
     </row>
-    <row r="177" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="177" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H177" t="s">
         <v>468</v>
       </c>
     </row>
-    <row r="178" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="178" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H178" t="s">
         <v>469</v>
       </c>
     </row>
-    <row r="179" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="179" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H179" t="s">
         <v>470</v>
       </c>
     </row>
-    <row r="180" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="180" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H180" t="s">
         <v>471</v>
       </c>
     </row>
-    <row r="181" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="181" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H181" t="s">
         <v>472</v>
       </c>
     </row>
-    <row r="182" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="182" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H182" t="s">
         <v>473</v>
       </c>
     </row>
-    <row r="183" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="183" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H183" t="s">
         <v>474</v>
       </c>
     </row>
-    <row r="184" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="184" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H184" t="s">
         <v>475</v>
       </c>
     </row>
-    <row r="185" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="185" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H185" t="s">
         <v>476</v>
       </c>
     </row>
-    <row r="186" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="186" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H186" t="s">
         <v>477</v>
       </c>
     </row>
-    <row r="187" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="187" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H187" t="s">
         <v>478</v>
       </c>
     </row>
-    <row r="188" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="188" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H188" t="s">
         <v>479</v>
       </c>
     </row>
-    <row r="189" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="189" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H189" t="s">
         <v>480</v>
       </c>
     </row>
-    <row r="190" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="190" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H190" t="s">
         <v>481</v>
       </c>
     </row>
-    <row r="191" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="191" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H191" t="s">
         <v>482</v>
       </c>
     </row>
-    <row r="192" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="192" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H192" t="s">
         <v>483</v>
       </c>
     </row>
-    <row r="193" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="193" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H193" t="s">
         <v>484</v>
       </c>
     </row>
-    <row r="194" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="194" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H194" t="s">
         <v>485</v>
       </c>
     </row>
-    <row r="195" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="195" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H195" t="s">
         <v>486</v>
       </c>
     </row>
-    <row r="196" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="196" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H196" t="s">
         <v>487</v>
       </c>
     </row>
-    <row r="197" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="197" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H197" t="s">
         <v>488</v>
       </c>
     </row>
-    <row r="198" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="198" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H198" t="s">
         <v>489</v>
       </c>
     </row>
-    <row r="199" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="199" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H199" t="s">
         <v>490</v>
       </c>
     </row>
-    <row r="200" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="200" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H200" t="s">
         <v>491</v>
       </c>
     </row>
-    <row r="201" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="201" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H201" t="s">
         <v>492</v>
       </c>
     </row>
-    <row r="202" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="202" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H202" t="s">
         <v>493</v>
       </c>
     </row>
-    <row r="203" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="203" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H203" t="s">
         <v>495</v>
       </c>
     </row>
-    <row r="204" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="204" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H204" t="s">
         <v>496</v>
       </c>
     </row>
-    <row r="205" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="205" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H205" t="s">
         <v>497</v>
       </c>
     </row>
-    <row r="206" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="206" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H206" t="s">
         <v>498</v>
       </c>
     </row>
-    <row r="207" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="207" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H207" t="s">
         <v>499</v>
       </c>
     </row>
-    <row r="208" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="208" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H208" t="s">
         <v>500</v>
       </c>
     </row>
-    <row r="209" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="209" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H209" t="s">
         <v>501</v>
       </c>
     </row>
-    <row r="210" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="210" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H210" t="s">
         <v>503</v>
       </c>
     </row>
-    <row r="211" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="211" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H211" t="s">
         <v>504</v>
       </c>
     </row>
-    <row r="212" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="212" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H212" t="s">
         <v>505</v>
       </c>
     </row>
-    <row r="213" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="213" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H213" t="s">
         <v>254</v>
       </c>
     </row>
-    <row r="214" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="214" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H214" t="s">
         <v>255</v>
       </c>
     </row>
-    <row r="215" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="215" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H215" t="s">
         <v>256</v>
       </c>
     </row>
-    <row r="216" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="216" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H216" t="s">
         <v>257</v>
       </c>
     </row>
-    <row r="217" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="217" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H217" t="s">
         <v>259</v>
       </c>
     </row>
-    <row r="218" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="218" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H218" t="s">
         <v>262</v>
       </c>
     </row>
-    <row r="219" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="219" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H219" t="s">
         <v>263</v>
       </c>
     </row>
-    <row r="220" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="220" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H220" t="s">
         <v>266</v>
       </c>
     </row>
-    <row r="221" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="221" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H221" t="s">
         <v>267</v>
       </c>
     </row>
-    <row r="222" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="222" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H222" t="s">
         <v>269</v>
       </c>
     </row>
-    <row r="223" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="223" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H223" t="s">
         <v>272</v>
       </c>
     </row>
-    <row r="224" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="224" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H224" t="s">
         <v>273</v>
       </c>
     </row>
-    <row r="225" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="225" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H225" t="s">
         <v>274</v>
       </c>
     </row>
-    <row r="226" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="226" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H226" t="s">
         <v>275</v>
       </c>
     </row>
-    <row r="227" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="227" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H227" t="s">
         <v>278</v>
       </c>
     </row>
-    <row r="228" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="228" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H228" t="s">
         <v>279</v>
       </c>
     </row>
-    <row r="229" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="229" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H229" t="s">
         <v>280</v>
       </c>
     </row>
-    <row r="230" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="230" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H230" t="s">
         <v>281</v>
       </c>
     </row>
-    <row r="231" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="231" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H231" t="s">
         <v>282</v>
       </c>
     </row>
-    <row r="232" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="232" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H232" t="s">
         <v>284</v>
       </c>
     </row>
-    <row r="233" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="233" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H233" t="s">
         <v>285</v>
       </c>
     </row>
-    <row r="234" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="234" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H234" t="s">
         <v>286</v>
       </c>
     </row>
-    <row r="235" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="235" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H235" t="s">
         <v>287</v>
       </c>
     </row>
-    <row r="236" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="236" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H236" t="s">
         <v>288</v>
       </c>
     </row>
-    <row r="237" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="237" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H237" t="s">
         <v>289</v>
       </c>
     </row>
-    <row r="238" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="238" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H238" t="s">
         <v>290</v>
       </c>
     </row>
-    <row r="239" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="239" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H239" t="s">
         <v>291</v>
       </c>
     </row>
-    <row r="240" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="240" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H240" t="s">
         <v>292</v>
       </c>
     </row>
-    <row r="241" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="241" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H241" t="s">
         <v>293</v>
       </c>
     </row>
-    <row r="242" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="242" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H242" t="s">
         <v>294</v>
       </c>
     </row>
-    <row r="243" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="243" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H243" t="s">
         <v>295</v>
       </c>
     </row>
-    <row r="244" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="244" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H244" t="s">
         <v>296</v>
       </c>
     </row>
-    <row r="245" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="245" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H245" t="s">
         <v>297</v>
       </c>
     </row>
-    <row r="246" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="246" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H246" t="s">
         <v>298</v>
       </c>
     </row>
-    <row r="247" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="247" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H247" t="s">
         <v>299</v>
       </c>
     </row>
-    <row r="248" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="248" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H248" t="s">
         <v>300</v>
       </c>
     </row>
-    <row r="249" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="249" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H249" t="s">
         <v>301</v>
       </c>
     </row>
-    <row r="250" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="250" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H250" t="s">
         <v>302</v>
       </c>
     </row>
-    <row r="251" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="251" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H251" t="s">
         <v>303</v>
       </c>
     </row>
-    <row r="252" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="252" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H252" t="s">
         <v>304</v>
       </c>
     </row>
-    <row r="253" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="253" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H253" t="s">
         <v>305</v>
       </c>
     </row>
-    <row r="254" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="254" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H254" t="s">
         <v>306</v>
       </c>
     </row>
-    <row r="255" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="255" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H255" t="s">
         <v>307</v>
       </c>
     </row>
-    <row r="256" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="256" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H256" t="s">
         <v>308</v>
       </c>
     </row>
-    <row r="257" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="257" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H257" t="s">
         <v>310</v>
       </c>
     </row>
-    <row r="258" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="258" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H258" t="s">
         <v>311</v>
       </c>
     </row>
-    <row r="259" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="259" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H259" t="s">
         <v>312</v>
       </c>
     </row>
-    <row r="260" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="260" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H260" t="s">
         <v>313</v>
       </c>
@@ -5880,9 +5877,9 @@
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B1" t="s">
         <v>194</v>
       </c>
@@ -5896,7 +5893,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>134</v>
       </c>
@@ -5913,7 +5910,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>135</v>
       </c>
@@ -5930,7 +5927,7 @@
         <v>1.595E-27</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>136</v>
       </c>
@@ -5947,7 +5944,7 @@
         <v>1.311E-14</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>137</v>
       </c>
@@ -5964,7 +5961,7 @@
         <v>1.3730000000000001E-3</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>138</v>
       </c>
@@ -5981,7 +5978,7 @@
         <v>1.034E-157</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>139</v>
       </c>
@@ -5998,7 +5995,7 @@
         <v>0.31790000000000002</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>140</v>
       </c>
@@ -6015,7 +6012,7 @@
         <v>5.3380000000000004E-9</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>141</v>
       </c>
@@ -6032,7 +6029,7 @@
         <v>7.597E-144</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>142</v>
       </c>
@@ -6049,7 +6046,7 @@
         <v>7.5620000000000003E-97</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>143</v>
       </c>
@@ -6066,7 +6063,7 @@
         <v>2.4479999999999999E-4</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>144</v>
       </c>
@@ -6083,7 +6080,7 @@
         <v>0.78369999999999995</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>145</v>
       </c>
@@ -6100,7 +6097,7 @@
         <v>0.89500000000000002</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>146</v>
       </c>
@@ -6117,7 +6114,7 @@
         <v>0.67849999999999999</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>147</v>
       </c>
@@ -6134,7 +6131,7 @@
         <v>0.89590000000000003</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>148</v>
       </c>
@@ -6151,7 +6148,7 @@
         <v>4.7519999999999997E-43</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>149</v>
       </c>
@@ -6168,7 +6165,7 @@
         <v>7.4689999999999998E-257</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>150</v>
       </c>
@@ -6185,7 +6182,7 @@
         <v>0.2155</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>186</v>
       </c>
@@ -6202,7 +6199,7 @@
         <v>4.0259999999999997E-2</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>187</v>
       </c>
@@ -6219,7 +6216,7 @@
         <v>3.721E-2</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>151</v>
       </c>
@@ -6236,7 +6233,7 @@
         <v>2.5340000000000001E-2</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>152</v>
       </c>
@@ -6253,7 +6250,7 @@
         <v>1.5990000000000001E-2</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>153</v>
       </c>
@@ -6270,7 +6267,7 @@
         <v>3.895E-78</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>154</v>
       </c>
@@ -6287,7 +6284,7 @@
         <v>0.99650000000000005</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>155</v>
       </c>
@@ -6304,7 +6301,7 @@
         <v>0.34179999999999999</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>156</v>
       </c>
@@ -6321,7 +6318,7 @@
         <v>1.623E-10</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>185</v>
       </c>
@@ -6338,7 +6335,7 @@
         <v>1.159E-8</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>157</v>
       </c>
@@ -6355,7 +6352,7 @@
         <v>6.82E-9</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>158</v>
       </c>
@@ -6372,7 +6369,7 @@
         <v>1.281E-56</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>159</v>
       </c>
@@ -6389,7 +6386,7 @@
         <v>0.58179999999999998</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>160</v>
       </c>
@@ -6406,7 +6403,7 @@
         <v>0.33389999999999997</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>161</v>
       </c>
@@ -6423,7 +6420,7 @@
         <v>2.7690000000000002E-46</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>162</v>
       </c>
@@ -6440,7 +6437,7 @@
         <v>5.3630000000000003E-36</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>163</v>
       </c>
@@ -6457,7 +6454,7 @@
         <v>2.178E-20</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>164</v>
       </c>
@@ -6474,7 +6471,7 @@
         <v>1.1529999999999999E-3</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>165</v>
       </c>
@@ -6491,7 +6488,7 @@
         <v>0.76480000000000004</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>166</v>
       </c>
@@ -6508,7 +6505,7 @@
         <v>0.29559999999999997</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>167</v>
       </c>
@@ -6525,7 +6522,7 @@
         <v>1.0739999999999999E-25</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>168</v>
       </c>
@@ -6542,7 +6539,7 @@
         <v>4.537E-111</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>169</v>
       </c>
@@ -6559,7 +6556,7 @@
         <v>0.68989999999999996</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>170</v>
       </c>
@@ -6576,7 +6573,7 @@
         <v>0.4456</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>188</v>
       </c>
@@ -6593,7 +6590,7 @@
         <v>3.175E-27</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>189</v>
       </c>
@@ -6610,7 +6607,7 @@
         <v>5.5849999999999999E-18</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>190</v>
       </c>
@@ -6627,7 +6624,7 @@
         <v>4.5689999999999999E-16</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>171</v>
       </c>
@@ -6644,7 +6641,7 @@
         <v>0.59089999999999998</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>172</v>
       </c>
@@ -6661,7 +6658,7 @@
         <v>1.1259999999999999E-2</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>173</v>
       </c>
@@ -6678,7 +6675,7 @@
         <v>0.54630000000000001</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>174</v>
       </c>
@@ -6695,7 +6692,7 @@
         <v>0.34620000000000001</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>175</v>
       </c>
@@ -6712,7 +6709,7 @@
         <v>3.1889999999999999E-19</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>176</v>
       </c>
@@ -6729,7 +6726,7 @@
         <v>3.4289999999999998E-7</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>177</v>
       </c>
@@ -6746,7 +6743,7 @@
         <v>0.77039999999999997</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>178</v>
       </c>
@@ -6763,7 +6760,7 @@
         <v>5.74E-39</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>179</v>
       </c>
@@ -6780,7 +6777,7 @@
         <v>2.0239999999999999E-66</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>180</v>
       </c>
@@ -6797,7 +6794,7 @@
         <v>4.929E-2</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>181</v>
       </c>
@@ -6814,7 +6811,7 @@
         <v>8.6540000000000003E-20</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>182</v>
       </c>
@@ -6831,7 +6828,7 @@
         <v>0.30409999999999998</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>183</v>
       </c>
@@ -6848,7 +6845,7 @@
         <v>1.3379999999999999E-27</v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>184</v>
       </c>
@@ -6876,7 +6873,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>